<commit_message>
Added Service and Presentation Layers
</commit_message>
<xml_diff>
--- a/Data base design/Database Design.xlsx
+++ b/Data base design/Database Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Talent500\Java\Coffee Case Study\CoffeeCaseStudy\Data base design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A840BA6-AEA6-4EFB-B1D7-68395FB01027}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A552C6A7-7B61-4DBB-A1F0-BB8093F13BE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database design" sheetId="1" r:id="rId1"/>
@@ -900,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD86299B-566D-4927-A3B4-5FCAD865A383}">
   <dimension ref="A1:XCG53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>